<commit_message>
update polyphone statistics - 越8d8a
</commit_message>
<xml_diff>
--- a/shc-hmogrph.xlsx
+++ b/shc-hmogrph.xlsx
@@ -5145,9 +5145,6 @@
     <t>8D8A</t>
   </si>
   <si>
-    <t>waiting for training</t>
-  </si>
-  <si>
     <t xml:space="preserve"> i53n 0.56(10)
  i34n 0.44(8)                                </t>
   </si>
@@ -5228,6 +5225,11 @@
   </si>
   <si>
     <t>3554/3596</t>
+  </si>
+  <si>
+    <t>h6h\\I:~12?{A} (92)
+h6h\\I:~12? (65)
+h6jo:~12? (0)</t>
   </si>
 </sst>
 </file>
@@ -5663,7 +5665,7 @@
   <dimension ref="A1:G59"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E4" sqref="E4"/>
+      <selection activeCell="F59" sqref="F59"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -5690,7 +5692,7 @@
         <v>4</v>
       </c>
       <c r="F1" s="13" t="s">
-        <v>1713</v>
+        <v>1712</v>
       </c>
       <c r="G1" s="8" t="s">
         <v>5</v>
@@ -5698,25 +5700,25 @@
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A2" s="13" t="s">
+        <v>1713</v>
+      </c>
+      <c r="B2" s="13" t="s">
         <v>1714</v>
       </c>
-      <c r="B2" s="13" t="s">
-        <v>1715</v>
-      </c>
       <c r="C2" s="13" t="s">
-        <v>1715</v>
+        <v>1714</v>
       </c>
       <c r="D2" s="13" t="s">
-        <v>1715</v>
+        <v>1714</v>
       </c>
       <c r="E2" s="13" t="s">
-        <v>1715</v>
+        <v>1714</v>
       </c>
       <c r="F2" s="23">
         <v>0.98829999999999996</v>
       </c>
       <c r="G2" s="13" t="s">
-        <v>1716</v>
+        <v>1715</v>
       </c>
     </row>
     <row r="3" spans="1:7" ht="25.5" x14ac:dyDescent="0.2">
@@ -6768,7 +6770,7 @@
         <v>9</v>
       </c>
       <c r="E48" s="11" t="s">
-        <v>1690</v>
+        <v>1689</v>
       </c>
       <c r="F48" s="16">
         <v>1</v>
@@ -7003,7 +7005,7 @@
         <v>1686</v>
       </c>
     </row>
-    <row r="59" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="59" spans="1:7" ht="38.25" x14ac:dyDescent="0.2">
       <c r="A59" s="8">
         <v>57</v>
       </c>
@@ -7013,13 +7015,17 @@
       <c r="C59" s="10" t="s">
         <v>1688</v>
       </c>
-      <c r="D59" s="10"/>
-      <c r="E59" s="11"/>
-      <c r="F59" s="12" t="s">
-        <v>1685</v>
+      <c r="D59" s="10">
+        <v>157</v>
+      </c>
+      <c r="E59" s="11" t="s">
+        <v>1716</v>
+      </c>
+      <c r="F59" s="14">
+        <v>0.98089999999999999</v>
       </c>
       <c r="G59" s="15" t="s">
-        <v>1689</v>
+        <v>1658</v>
       </c>
     </row>
   </sheetData>
@@ -14215,7 +14221,7 @@
         <v>476</v>
       </c>
       <c r="B478" s="22" t="s">
-        <v>1691</v>
+        <v>1690</v>
       </c>
       <c r="C478" s="6" t="s">
         <v>144</v>
@@ -15940,13 +15946,13 @@
         <v>591</v>
       </c>
       <c r="B593" s="18" t="s">
+        <v>1691</v>
+      </c>
+      <c r="C593" s="18" t="s">
         <v>1692</v>
       </c>
-      <c r="C593" s="18" t="s">
-        <v>1693</v>
-      </c>
       <c r="D593" s="13" t="s">
-        <v>1712</v>
+        <v>1711</v>
       </c>
       <c r="E593" s="11"/>
       <c r="F593" s="19"/>
@@ -15957,13 +15963,13 @@
         <v>592</v>
       </c>
       <c r="B594" s="18" t="s">
+        <v>1693</v>
+      </c>
+      <c r="C594" s="18" t="s">
         <v>1694</v>
       </c>
-      <c r="C594" s="18" t="s">
-        <v>1695</v>
-      </c>
       <c r="D594" s="13" t="s">
-        <v>1712</v>
+        <v>1711</v>
       </c>
       <c r="E594" s="11"/>
       <c r="F594" s="19"/>
@@ -15974,13 +15980,13 @@
         <v>593</v>
       </c>
       <c r="B595" s="18" t="s">
+        <v>1695</v>
+      </c>
+      <c r="C595" s="18" t="s">
         <v>1696</v>
       </c>
-      <c r="C595" s="18" t="s">
-        <v>1697</v>
-      </c>
       <c r="D595" s="13" t="s">
-        <v>1712</v>
+        <v>1711</v>
       </c>
       <c r="E595" s="11"/>
       <c r="F595" s="19"/>
@@ -15991,13 +15997,13 @@
         <v>594</v>
       </c>
       <c r="B596" s="18" t="s">
+        <v>1697</v>
+      </c>
+      <c r="C596" s="18" t="s">
         <v>1698</v>
       </c>
-      <c r="C596" s="18" t="s">
-        <v>1699</v>
-      </c>
       <c r="D596" s="13" t="s">
-        <v>1712</v>
+        <v>1711</v>
       </c>
       <c r="E596" s="11"/>
       <c r="F596" s="19"/>
@@ -16008,13 +16014,13 @@
         <v>595</v>
       </c>
       <c r="B597" s="18" t="s">
+        <v>1699</v>
+      </c>
+      <c r="C597" s="18" t="s">
         <v>1700</v>
       </c>
-      <c r="C597" s="18" t="s">
-        <v>1701</v>
-      </c>
       <c r="D597" s="13" t="s">
-        <v>1712</v>
+        <v>1711</v>
       </c>
       <c r="E597" s="11"/>
       <c r="F597" s="19"/>
@@ -16025,13 +16031,13 @@
         <v>596</v>
       </c>
       <c r="B598" s="18" t="s">
+        <v>1701</v>
+      </c>
+      <c r="C598" s="18" t="s">
         <v>1702</v>
       </c>
-      <c r="C598" s="18" t="s">
-        <v>1703</v>
-      </c>
       <c r="D598" s="13" t="s">
-        <v>1712</v>
+        <v>1711</v>
       </c>
       <c r="E598" s="11"/>
       <c r="F598" s="19"/>
@@ -16042,13 +16048,13 @@
         <v>597</v>
       </c>
       <c r="B599" s="18" t="s">
+        <v>1703</v>
+      </c>
+      <c r="C599" s="18" t="s">
         <v>1704</v>
       </c>
-      <c r="C599" s="18" t="s">
-        <v>1705</v>
-      </c>
       <c r="D599" s="13" t="s">
-        <v>1712</v>
+        <v>1711</v>
       </c>
       <c r="E599" s="11"/>
       <c r="F599" s="19"/>
@@ -16059,13 +16065,13 @@
         <v>598</v>
       </c>
       <c r="B600" s="18" t="s">
+        <v>1705</v>
+      </c>
+      <c r="C600" s="18" t="s">
         <v>1706</v>
       </c>
-      <c r="C600" s="18" t="s">
-        <v>1707</v>
-      </c>
       <c r="D600" s="13" t="s">
-        <v>1712</v>
+        <v>1711</v>
       </c>
       <c r="E600" s="11"/>
       <c r="F600" s="19"/>
@@ -16076,13 +16082,13 @@
         <v>599</v>
       </c>
       <c r="B601" s="18" t="s">
+        <v>1707</v>
+      </c>
+      <c r="C601" s="18" t="s">
         <v>1708</v>
       </c>
-      <c r="C601" s="18" t="s">
-        <v>1709</v>
-      </c>
       <c r="D601" s="13" t="s">
-        <v>1712</v>
+        <v>1711</v>
       </c>
       <c r="E601" s="11"/>
       <c r="F601" s="12"/>
@@ -16093,13 +16099,13 @@
         <v>600</v>
       </c>
       <c r="B602" s="13" t="s">
+        <v>1709</v>
+      </c>
+      <c r="C602" s="20" t="s">
         <v>1710</v>
       </c>
-      <c r="C602" s="20" t="s">
+      <c r="D602" s="13" t="s">
         <v>1711</v>
-      </c>
-      <c r="D602" s="13" t="s">
-        <v>1712</v>
       </c>
       <c r="E602" s="21"/>
       <c r="F602" s="12"/>

</xml_diff>

<commit_message>
add 8fd8 还  Polyphone
</commit_message>
<xml_diff>
--- a/shc-hmogrph.xlsx
+++ b/shc-hmogrph.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2089" uniqueCount="1717">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2089" uniqueCount="1716">
   <si>
     <t>No</t>
   </si>
@@ -5133,12 +5133,6 @@
     <t>8FD8</t>
   </si>
   <si>
-    <t>waiting</t>
-  </si>
-  <si>
-    <t>need labelling</t>
-  </si>
-  <si>
     <t>越</t>
   </si>
   <si>
@@ -5230,6 +5224,10 @@
     <t>h6h\\I:~12?{A} (92)
 h6h\\I:~12? (65)
 h6jo:~12? (0)</t>
+  </si>
+  <si>
+    <t>h6we23 (94)
+h6e23{VA} (730)</t>
   </si>
 </sst>
 </file>
@@ -5664,8 +5662,8 @@
   </sheetPr>
   <dimension ref="A1:G59"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F59" sqref="F59"/>
+    <sheetView tabSelected="1" topLeftCell="A40" workbookViewId="0">
+      <selection activeCell="K47" sqref="K47"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -5692,7 +5690,7 @@
         <v>4</v>
       </c>
       <c r="F1" s="13" t="s">
-        <v>1712</v>
+        <v>1710</v>
       </c>
       <c r="G1" s="8" t="s">
         <v>5</v>
@@ -5700,25 +5698,25 @@
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A2" s="13" t="s">
-        <v>1713</v>
+        <v>1711</v>
       </c>
       <c r="B2" s="13" t="s">
-        <v>1714</v>
+        <v>1712</v>
       </c>
       <c r="C2" s="13" t="s">
-        <v>1714</v>
+        <v>1712</v>
       </c>
       <c r="D2" s="13" t="s">
-        <v>1714</v>
+        <v>1712</v>
       </c>
       <c r="E2" s="13" t="s">
-        <v>1714</v>
+        <v>1712</v>
       </c>
       <c r="F2" s="23">
         <v>0.98829999999999996</v>
       </c>
       <c r="G2" s="13" t="s">
-        <v>1715</v>
+        <v>1713</v>
       </c>
     </row>
     <row r="3" spans="1:7" ht="25.5" x14ac:dyDescent="0.2">
@@ -6770,7 +6768,7 @@
         <v>9</v>
       </c>
       <c r="E48" s="11" t="s">
-        <v>1689</v>
+        <v>1687</v>
       </c>
       <c r="F48" s="16">
         <v>1</v>
@@ -6986,7 +6984,7 @@
         <v>1658</v>
       </c>
     </row>
-    <row r="58" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="58" spans="1:7" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A58" s="8">
         <v>56</v>
       </c>
@@ -6996,13 +6994,17 @@
       <c r="C58" s="10" t="s">
         <v>1684</v>
       </c>
-      <c r="D58" s="10"/>
-      <c r="E58" s="11"/>
-      <c r="F58" s="12" t="s">
-        <v>1685</v>
+      <c r="D58" s="10">
+        <v>824</v>
+      </c>
+      <c r="E58" s="11" t="s">
+        <v>1715</v>
+      </c>
+      <c r="F58" s="14">
+        <v>0.99270000000000003</v>
       </c>
       <c r="G58" s="15" t="s">
-        <v>1686</v>
+        <v>1658</v>
       </c>
     </row>
     <row r="59" spans="1:7" ht="38.25" x14ac:dyDescent="0.2">
@@ -7010,16 +7012,16 @@
         <v>57</v>
       </c>
       <c r="B59" s="10" t="s">
-        <v>1687</v>
+        <v>1685</v>
       </c>
       <c r="C59" s="10" t="s">
-        <v>1688</v>
+        <v>1686</v>
       </c>
       <c r="D59" s="10">
         <v>157</v>
       </c>
       <c r="E59" s="11" t="s">
-        <v>1716</v>
+        <v>1714</v>
       </c>
       <c r="F59" s="14">
         <v>0.98089999999999999</v>
@@ -14221,7 +14223,7 @@
         <v>476</v>
       </c>
       <c r="B478" s="22" t="s">
-        <v>1690</v>
+        <v>1688</v>
       </c>
       <c r="C478" s="6" t="s">
         <v>144</v>
@@ -15946,13 +15948,13 @@
         <v>591</v>
       </c>
       <c r="B593" s="18" t="s">
-        <v>1691</v>
+        <v>1689</v>
       </c>
       <c r="C593" s="18" t="s">
-        <v>1692</v>
+        <v>1690</v>
       </c>
       <c r="D593" s="13" t="s">
-        <v>1711</v>
+        <v>1709</v>
       </c>
       <c r="E593" s="11"/>
       <c r="F593" s="19"/>
@@ -15963,13 +15965,13 @@
         <v>592</v>
       </c>
       <c r="B594" s="18" t="s">
-        <v>1693</v>
+        <v>1691</v>
       </c>
       <c r="C594" s="18" t="s">
-        <v>1694</v>
+        <v>1692</v>
       </c>
       <c r="D594" s="13" t="s">
-        <v>1711</v>
+        <v>1709</v>
       </c>
       <c r="E594" s="11"/>
       <c r="F594" s="19"/>
@@ -15980,13 +15982,13 @@
         <v>593</v>
       </c>
       <c r="B595" s="18" t="s">
-        <v>1695</v>
+        <v>1693</v>
       </c>
       <c r="C595" s="18" t="s">
-        <v>1696</v>
+        <v>1694</v>
       </c>
       <c r="D595" s="13" t="s">
-        <v>1711</v>
+        <v>1709</v>
       </c>
       <c r="E595" s="11"/>
       <c r="F595" s="19"/>
@@ -15997,13 +15999,13 @@
         <v>594</v>
       </c>
       <c r="B596" s="18" t="s">
-        <v>1697</v>
+        <v>1695</v>
       </c>
       <c r="C596" s="18" t="s">
-        <v>1698</v>
+        <v>1696</v>
       </c>
       <c r="D596" s="13" t="s">
-        <v>1711</v>
+        <v>1709</v>
       </c>
       <c r="E596" s="11"/>
       <c r="F596" s="19"/>
@@ -16014,13 +16016,13 @@
         <v>595</v>
       </c>
       <c r="B597" s="18" t="s">
-        <v>1699</v>
+        <v>1697</v>
       </c>
       <c r="C597" s="18" t="s">
-        <v>1700</v>
+        <v>1698</v>
       </c>
       <c r="D597" s="13" t="s">
-        <v>1711</v>
+        <v>1709</v>
       </c>
       <c r="E597" s="11"/>
       <c r="F597" s="19"/>
@@ -16031,13 +16033,13 @@
         <v>596</v>
       </c>
       <c r="B598" s="18" t="s">
-        <v>1701</v>
+        <v>1699</v>
       </c>
       <c r="C598" s="18" t="s">
-        <v>1702</v>
+        <v>1700</v>
       </c>
       <c r="D598" s="13" t="s">
-        <v>1711</v>
+        <v>1709</v>
       </c>
       <c r="E598" s="11"/>
       <c r="F598" s="19"/>
@@ -16048,13 +16050,13 @@
         <v>597</v>
       </c>
       <c r="B599" s="18" t="s">
-        <v>1703</v>
+        <v>1701</v>
       </c>
       <c r="C599" s="18" t="s">
-        <v>1704</v>
+        <v>1702</v>
       </c>
       <c r="D599" s="13" t="s">
-        <v>1711</v>
+        <v>1709</v>
       </c>
       <c r="E599" s="11"/>
       <c r="F599" s="19"/>
@@ -16065,13 +16067,13 @@
         <v>598</v>
       </c>
       <c r="B600" s="18" t="s">
-        <v>1705</v>
+        <v>1703</v>
       </c>
       <c r="C600" s="18" t="s">
-        <v>1706</v>
+        <v>1704</v>
       </c>
       <c r="D600" s="13" t="s">
-        <v>1711</v>
+        <v>1709</v>
       </c>
       <c r="E600" s="11"/>
       <c r="F600" s="19"/>
@@ -16082,13 +16084,13 @@
         <v>599</v>
       </c>
       <c r="B601" s="18" t="s">
-        <v>1707</v>
+        <v>1705</v>
       </c>
       <c r="C601" s="18" t="s">
-        <v>1708</v>
+        <v>1706</v>
       </c>
       <c r="D601" s="13" t="s">
-        <v>1711</v>
+        <v>1709</v>
       </c>
       <c r="E601" s="11"/>
       <c r="F601" s="12"/>
@@ -16099,13 +16101,13 @@
         <v>600</v>
       </c>
       <c r="B602" s="13" t="s">
+        <v>1707</v>
+      </c>
+      <c r="C602" s="20" t="s">
+        <v>1708</v>
+      </c>
+      <c r="D602" s="13" t="s">
         <v>1709</v>
-      </c>
-      <c r="C602" s="20" t="s">
-        <v>1710</v>
-      </c>
-      <c r="D602" s="13" t="s">
-        <v>1711</v>
       </c>
       <c r="E602" s="21"/>
       <c r="F602" s="12"/>

</xml_diff>